<commit_message>
final work log update
final entries (yay)
</commit_message>
<xml_diff>
--- a/Work Logs/Work Log Spreadsheet - Jonathan Mak.xlsx
+++ b/Work Logs/Work Log Spreadsheet - Jonathan Mak.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -152,6 +152,33 @@
   </si>
   <si>
     <t>analyzed Piazza, coursespaces. Wrote results for final report</t>
+  </si>
+  <si>
+    <t>Week 8</t>
+  </si>
+  <si>
+    <t>Nov 30th</t>
+  </si>
+  <si>
+    <t>group meeting for presentation slides</t>
+  </si>
+  <si>
+    <t>Dec 3rd</t>
+  </si>
+  <si>
+    <t>group meeting to delegate final paper tasks, first pass at editing</t>
+  </si>
+  <si>
+    <t>Dec 4th</t>
+  </si>
+  <si>
+    <t>fixed citation numbers, more general editing</t>
+  </si>
+  <si>
+    <t>Dec 5th</t>
+  </si>
+  <si>
+    <t>final editing pass</t>
   </si>
 </sst>
 </file>
@@ -499,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -748,6 +775,53 @@
         <v>2</v>
       </c>
     </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="1">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A4:A6"/>

</xml_diff>